<commit_message>
updated logics for: MetroE MegaPop (CE)
</commit_message>
<xml_diff>
--- a/scripts/reports/gsp_transport/resource/mapping_table_new.xlsx
+++ b/scripts/reports/gsp_transport/resource/mapping_table_new.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\p1319639\Development\orion_report_management_tool\scripts\reports\gsp_transport\resource\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{60CBDF94-B692-4151-AAC0-CA9B120456CE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{49110EBD-7910-494F-806C-5DEF41ED1156}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-47520" yWindow="-7935" windowWidth="21600" windowHeight="11265" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-16320" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="mapping_table_new" sheetId="1" r:id="rId1"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="39">
   <si>
     <t>Service</t>
   </si>
@@ -156,6 +156,13 @@
 GSDT Co-ordination Wrk-BQ
 GSDT Co-ordination WK-BQ</t>
   </si>
+  <si>
+    <t>Yes if Co-ordination queue is not COM 
+and customer is SINGNET</t>
+  </si>
+  <si>
+    <t>Yes and copy to Co-ordination columns</t>
+  </si>
 </sst>
 </file>
 
@@ -303,7 +310,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="33">
+  <fills count="34">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -481,6 +488,12 @@
       <patternFill patternType="solid">
         <fgColor theme="9" tint="0.39997558519241921"/>
         <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
@@ -696,11 +709,38 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="33" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="33" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -708,29 +748,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
@@ -741,6 +763,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="33" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="33" borderId="13" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1097,10 +1121,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:J15"/>
+  <dimension ref="A1:J17"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="G23" sqref="G23"/>
+      <selection activeCell="I11" sqref="I11:I12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1111,7 +1135,7 @@
     <col min="4" max="4" width="14.54296875" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="27.81640625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="23.453125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="9.08984375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="35.1796875" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="27.36328125" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="24.90625" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="9.08984375" bestFit="1" customWidth="1"/>
@@ -1148,13 +1172,13 @@
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A2" s="5" t="s">
+      <c r="A2" s="16" t="s">
         <v>6</v>
       </c>
-      <c r="B2" s="6" t="s">
+      <c r="B2" s="17" t="s">
         <v>6</v>
       </c>
-      <c r="C2" s="7" t="s">
+      <c r="C2" s="14" t="s">
         <v>29</v>
       </c>
       <c r="D2" s="1" t="s">
@@ -1180,9 +1204,9 @@
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A3" s="5"/>
-      <c r="B3" s="8"/>
-      <c r="C3" s="4"/>
+      <c r="A3" s="16"/>
+      <c r="B3" s="18"/>
+      <c r="C3" s="15"/>
       <c r="D3" s="1" t="s">
         <v>11</v>
       </c>
@@ -1206,19 +1230,19 @@
       </c>
     </row>
     <row r="4" spans="1:10" ht="29" x14ac:dyDescent="0.35">
-      <c r="A4" s="5"/>
-      <c r="B4" s="9"/>
-      <c r="C4" s="4"/>
+      <c r="A4" s="16"/>
+      <c r="B4" s="19"/>
+      <c r="C4" s="15"/>
       <c r="D4" s="1" t="s">
         <v>12</v>
       </c>
       <c r="E4" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="F4" s="10" t="s">
+      <c r="F4" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="G4" s="10" t="s">
+      <c r="G4" s="4" t="s">
         <v>27</v>
       </c>
       <c r="H4" s="1" t="s">
@@ -1231,20 +1255,20 @@
         <v>26</v>
       </c>
     </row>
-    <row r="5" spans="1:10" ht="29" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A5" s="5" t="s">
+    <row r="5" spans="1:10" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A5" s="16" t="s">
         <v>13</v>
       </c>
-      <c r="B5" s="6" t="s">
+      <c r="B5" s="17" t="s">
         <v>13</v>
       </c>
-      <c r="C5" s="5" t="s">
+      <c r="C5" s="16" t="s">
         <v>14</v>
       </c>
-      <c r="D5" s="11" t="s">
+      <c r="D5" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="E5" s="11" t="s">
+      <c r="E5" s="8" t="s">
         <v>8</v>
       </c>
       <c r="F5" s="1" t="s">
@@ -1253,78 +1277,68 @@
       <c r="G5" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="H5" s="2" t="s">
+      <c r="H5" s="10" t="s">
         <v>8</v>
       </c>
       <c r="I5" s="12" t="s">
         <v>21</v>
       </c>
-      <c r="J5" s="2" t="s">
+      <c r="J5" s="10" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A6" s="5"/>
-      <c r="B6" s="8"/>
-      <c r="C6" s="5"/>
-      <c r="D6" s="13"/>
-      <c r="E6" s="13"/>
-      <c r="F6" s="1" t="s">
+    <row r="6" spans="1:10" ht="32.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A6" s="16"/>
+      <c r="B6" s="18"/>
+      <c r="C6" s="16"/>
+      <c r="D6" s="9"/>
+      <c r="E6" s="9"/>
+      <c r="F6" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="G6" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="H6" s="3"/>
-      <c r="I6" s="14"/>
-      <c r="J6" s="3"/>
+      <c r="G6" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="H6" s="11"/>
+      <c r="I6" s="13"/>
+      <c r="J6" s="11"/>
     </row>
     <row r="7" spans="1:10" ht="29" x14ac:dyDescent="0.35">
-      <c r="A7" s="5"/>
-      <c r="B7" s="8"/>
-      <c r="C7" s="5"/>
-      <c r="D7" s="1" t="s">
+      <c r="A7" s="16"/>
+      <c r="B7" s="18"/>
+      <c r="C7" s="16"/>
+      <c r="D7" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="E7" s="1" t="s">
+      <c r="E7" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="F7" s="10" t="s">
+      <c r="F7" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="G7" s="10" t="s">
+      <c r="G7" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="H7" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="I7" s="10" t="s">
-        <v>21</v>
-      </c>
-      <c r="J7" s="1" t="s">
-        <v>26</v>
-      </c>
+      <c r="H7" s="2"/>
+      <c r="I7" s="5"/>
+      <c r="J7" s="2"/>
     </row>
     <row r="8" spans="1:10" ht="29" x14ac:dyDescent="0.35">
-      <c r="A8" s="5"/>
-      <c r="B8" s="9"/>
-      <c r="C8" s="5"/>
-      <c r="D8" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="E8" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="F8" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="G8" s="10" t="s">
-        <v>27</v>
+      <c r="A8" s="16"/>
+      <c r="B8" s="18"/>
+      <c r="C8" s="16"/>
+      <c r="D8" s="9"/>
+      <c r="E8" s="9"/>
+      <c r="F8" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="G8" s="7" t="s">
+        <v>37</v>
       </c>
       <c r="H8" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="I8" s="10" t="s">
+      <c r="I8" s="4" t="s">
         <v>21</v>
       </c>
       <c r="J8" s="1" t="s">
@@ -1332,184 +1346,230 @@
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A9" s="6" t="s">
+      <c r="A9" s="16"/>
+      <c r="B9" s="18"/>
+      <c r="C9" s="16"/>
+      <c r="D9" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="E9" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="F9" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="G9" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="H9" s="3"/>
+      <c r="I9" s="4"/>
+      <c r="J9" s="3"/>
+    </row>
+    <row r="10" spans="1:10" ht="29" x14ac:dyDescent="0.35">
+      <c r="A10" s="16"/>
+      <c r="B10" s="19"/>
+      <c r="C10" s="16"/>
+      <c r="D10" s="9"/>
+      <c r="E10" s="9"/>
+      <c r="F10" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="G10" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="H10" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="I10" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="J10" s="1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A11" s="17" t="s">
         <v>16</v>
       </c>
-      <c r="B9" s="6" t="s">
+      <c r="B11" s="17" t="s">
         <v>28</v>
       </c>
-      <c r="C9" s="15" t="s">
+      <c r="C11" s="20" t="s">
         <v>33</v>
       </c>
-      <c r="D9" s="2" t="s">
+      <c r="D11" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="E9" s="1" t="s">
+      <c r="E11" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="F9" s="1" t="s">
+      <c r="F11" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="G9" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="H9" s="2"/>
-      <c r="I9" s="12"/>
-      <c r="J9" s="2"/>
-    </row>
-    <row r="10" spans="1:10" ht="29" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A10" s="8"/>
-      <c r="B10" s="8"/>
-      <c r="C10" s="16"/>
-      <c r="D10" s="3"/>
-      <c r="E10" s="1" t="s">
+      <c r="G11" s="23" t="s">
+        <v>38</v>
+      </c>
+      <c r="H11" s="10"/>
+      <c r="I11" s="12"/>
+      <c r="J11" s="10"/>
+    </row>
+    <row r="12" spans="1:10" ht="29" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A12" s="18"/>
+      <c r="B12" s="18"/>
+      <c r="C12" s="21"/>
+      <c r="D12" s="11"/>
+      <c r="E12" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="F10" s="1" t="s">
+      <c r="F12" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="G10" s="3"/>
-      <c r="H10" s="3"/>
-      <c r="I10" s="14"/>
-      <c r="J10" s="3"/>
-    </row>
-    <row r="11" spans="1:10" ht="47" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A11" s="8"/>
-      <c r="B11" s="8"/>
-      <c r="C11" s="16"/>
-      <c r="D11" s="1" t="s">
+      <c r="G12" s="24"/>
+      <c r="H12" s="11"/>
+      <c r="I12" s="13"/>
+      <c r="J12" s="11"/>
+    </row>
+    <row r="13" spans="1:10" ht="47" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A13" s="18"/>
+      <c r="B13" s="18"/>
+      <c r="C13" s="21"/>
+      <c r="D13" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="E11" s="1" t="s">
+      <c r="E13" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="F11" s="10" t="s">
+      <c r="F13" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="G11" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="H11" s="1"/>
-      <c r="I11" s="1"/>
-      <c r="J11" s="1"/>
-    </row>
-    <row r="12" spans="1:10" ht="55" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A12" s="9"/>
-      <c r="B12" s="9"/>
-      <c r="C12" s="17"/>
-      <c r="D12" s="1" t="s">
+      <c r="G13" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="H13" s="1"/>
+      <c r="I13" s="1"/>
+      <c r="J13" s="1"/>
+    </row>
+    <row r="14" spans="1:10" ht="55" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A14" s="19"/>
+      <c r="B14" s="19"/>
+      <c r="C14" s="22"/>
+      <c r="D14" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="E12" s="1" t="s">
+      <c r="E14" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="F12" s="1" t="s">
+      <c r="F14" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="G12" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="H12" s="1"/>
-      <c r="I12" s="1"/>
-      <c r="J12" s="1"/>
-    </row>
-    <row r="13" spans="1:10" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A13" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="B13" s="6" t="s">
-        <v>18</v>
-      </c>
-      <c r="C13" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="D13" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="E13" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="F13" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="G13" s="10" t="s">
-        <v>27</v>
-      </c>
-      <c r="H13" s="10" t="s">
-        <v>31</v>
-      </c>
-      <c r="I13" s="10" t="s">
-        <v>36</v>
-      </c>
-      <c r="J13" s="1" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A14" s="5"/>
-      <c r="B14" s="8"/>
-      <c r="C14" s="5"/>
-      <c r="D14" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="E14" s="1"/>
-      <c r="F14" s="1"/>
-      <c r="G14" s="1"/>
+      <c r="G14" s="6" t="s">
+        <v>38</v>
+      </c>
       <c r="H14" s="1"/>
       <c r="I14" s="1"/>
       <c r="J14" s="1"/>
     </row>
     <row r="15" spans="1:10" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A15" s="5"/>
-      <c r="B15" s="9"/>
-      <c r="C15" s="5"/>
+      <c r="A15" s="16" t="s">
+        <v>18</v>
+      </c>
+      <c r="B15" s="17" t="s">
+        <v>18</v>
+      </c>
+      <c r="C15" s="16" t="s">
+        <v>19</v>
+      </c>
       <c r="D15" s="1" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>20</v>
+        <v>8</v>
       </c>
       <c r="F15" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="G15" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="G15" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="H15" s="10" t="s">
-        <v>32</v>
-      </c>
-      <c r="I15" s="10" t="s">
+      <c r="H15" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="I15" s="4" t="s">
         <v>36</v>
       </c>
       <c r="J15" s="1" t="s">
         <v>26</v>
       </c>
     </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A16" s="16"/>
+      <c r="B16" s="18"/>
+      <c r="C16" s="16"/>
+      <c r="D16" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E16" s="1"/>
+      <c r="F16" s="1"/>
+      <c r="G16" s="1"/>
+      <c r="H16" s="1"/>
+      <c r="I16" s="1"/>
+      <c r="J16" s="1"/>
+    </row>
+    <row r="17" spans="1:10" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A17" s="16"/>
+      <c r="B17" s="19"/>
+      <c r="C17" s="16"/>
+      <c r="D17" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E17" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="F17" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="G17" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="H17" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="I17" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="J17" s="1" t="s">
+        <v>26</v>
+      </c>
+    </row>
   </sheetData>
   <autoFilter ref="A1:J1" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
-  <mergeCells count="22">
-    <mergeCell ref="I9:I10"/>
-    <mergeCell ref="J9:J10"/>
-    <mergeCell ref="D9:D10"/>
-    <mergeCell ref="A9:A12"/>
-    <mergeCell ref="B9:B12"/>
-    <mergeCell ref="G9:G10"/>
-    <mergeCell ref="H9:H10"/>
-    <mergeCell ref="C2:C4"/>
-    <mergeCell ref="C5:C8"/>
-    <mergeCell ref="C13:C15"/>
+  <mergeCells count="26">
+    <mergeCell ref="I11:I12"/>
+    <mergeCell ref="J11:J12"/>
+    <mergeCell ref="D11:D12"/>
+    <mergeCell ref="A11:A14"/>
+    <mergeCell ref="B11:B14"/>
+    <mergeCell ref="G11:G12"/>
+    <mergeCell ref="H11:H12"/>
+    <mergeCell ref="C15:C17"/>
     <mergeCell ref="A2:A4"/>
-    <mergeCell ref="A5:A8"/>
-    <mergeCell ref="A13:A15"/>
+    <mergeCell ref="A5:A10"/>
+    <mergeCell ref="A15:A17"/>
     <mergeCell ref="B2:B4"/>
-    <mergeCell ref="B5:B8"/>
-    <mergeCell ref="B13:B15"/>
-    <mergeCell ref="C9:C12"/>
-    <mergeCell ref="D5:D6"/>
-    <mergeCell ref="E5:E6"/>
+    <mergeCell ref="B5:B10"/>
+    <mergeCell ref="B15:B17"/>
+    <mergeCell ref="C11:C14"/>
     <mergeCell ref="H5:H6"/>
     <mergeCell ref="I5:I6"/>
     <mergeCell ref="J5:J6"/>
+    <mergeCell ref="C2:C4"/>
+    <mergeCell ref="C5:C10"/>
+    <mergeCell ref="D7:D8"/>
+    <mergeCell ref="E7:E8"/>
+    <mergeCell ref="D9:D10"/>
+    <mergeCell ref="E9:E10"/>
+    <mergeCell ref="D5:D6"/>
+    <mergeCell ref="E5:E6"/>
   </mergeCells>
   <phoneticPr fontId="18" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
support for ELK0003 and "Node & Cct Deletion (DN)"
</commit_message>
<xml_diff>
--- a/scripts/reports/gsp_transport/resource/mapping_table_new.xlsx
+++ b/scripts/reports/gsp_transport/resource/mapping_table_new.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\p1319639\Development\orion_report_management_tool\scripts\reports\gsp_transport\resource\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CC534D47-F60C-49E8-98F6-7DF9C8677940}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6FD5BF23-5F4C-4C4B-A4DA-7BD2C3D2EB1E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="25800" yWindow="-21600" windowWidth="25800" windowHeight="21000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="39">
   <si>
     <t>Service</t>
   </si>
@@ -137,6 +137,31 @@
     <t>GSDT31
 ODC_xxx
 RDC_xxx</t>
+  </si>
+  <si>
+    <t>GSPSG_ME</t>
+  </si>
+  <si>
+    <t>Circuit Configuration-STM</t>
+  </si>
+  <si>
+    <t>GSDT Co-ordination Work
+GSDT Co-ordination Wrk-BQ
+GSDT Co-ordination WK-BQ</t>
+  </si>
+  <si>
+    <t>Yes if Co-ordination queue is not COM 
+and customer is SINGNET</t>
+  </si>
+  <si>
+    <t>Yes and copy to Co-ordination columns</t>
+  </si>
+  <si>
+    <t>has COM date</t>
+  </si>
+  <si>
+    <t>Node &amp; Circuit Deletion
+Node &amp; Cct Deletion (DN)</t>
   </si>
   <si>
     <t>ELK0031
@@ -148,28 +173,8 @@
 ELK0091
 ELK0092
 ELK0093
-ELK0094</t>
-  </si>
-  <si>
-    <t>GSPSG_ME</t>
-  </si>
-  <si>
-    <t>Circuit Configuration-STM</t>
-  </si>
-  <si>
-    <t>GSDT Co-ordination Work
-GSDT Co-ordination Wrk-BQ
-GSDT Co-ordination WK-BQ</t>
-  </si>
-  <si>
-    <t>Yes if Co-ordination queue is not COM 
-and customer is SINGNET</t>
-  </si>
-  <si>
-    <t>Yes and copy to Co-ordination columns</t>
-  </si>
-  <si>
-    <t>has COM date</t>
+ELK0094
+ELK0003</t>
   </si>
 </sst>
 </file>
@@ -743,12 +748,6 @@
     <xf numFmtId="0" fontId="0" fillId="34" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -757,8 +756,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -769,6 +768,17 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="33" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="33" borderId="13" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -777,11 +787,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="33" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="33" borderId="13" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="42">
@@ -1175,7 +1180,7 @@
         <v>4</v>
       </c>
       <c r="F1" s="8" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="G1" s="1" t="s">
         <v>5</v>
@@ -1184,20 +1189,20 @@
         <v>4</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A2" s="18" t="s">
+      <c r="A2" s="16" t="s">
         <v>6</v>
       </c>
-      <c r="B2" s="15" t="s">
+      <c r="B2" s="13" t="s">
         <v>27</v>
       </c>
-      <c r="C2" s="11" t="s">
+      <c r="C2" s="21" t="s">
         <v>7</v>
       </c>
-      <c r="D2" s="11" t="s">
+      <c r="D2" s="21" t="s">
         <v>8</v>
       </c>
       <c r="E2" s="8" t="s">
@@ -1206,38 +1211,38 @@
       <c r="F2" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="G2" s="13" t="s">
+      <c r="G2" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="H2" s="13" t="s">
+      <c r="H2" s="11" t="s">
         <v>10</v>
       </c>
       <c r="I2" s="8"/>
     </row>
     <row r="3" spans="1:9" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="19"/>
-      <c r="B3" s="26"/>
-      <c r="C3" s="12"/>
-      <c r="D3" s="12"/>
+      <c r="A3" s="17"/>
+      <c r="B3" s="15"/>
+      <c r="C3" s="22"/>
+      <c r="D3" s="22"/>
       <c r="E3" s="9" t="s">
         <v>9</v>
       </c>
       <c r="F3" s="10" t="s">
-        <v>35</v>
-      </c>
-      <c r="G3" s="14"/>
-      <c r="H3" s="14"/>
+        <v>34</v>
+      </c>
+      <c r="G3" s="12"/>
+      <c r="H3" s="12"/>
       <c r="I3" s="1" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A4" s="19"/>
-      <c r="B4" s="26"/>
-      <c r="C4" s="11" t="s">
+      <c r="A4" s="17"/>
+      <c r="B4" s="15"/>
+      <c r="C4" s="21" t="s">
         <v>11</v>
       </c>
-      <c r="D4" s="11" t="s">
+      <c r="D4" s="21" t="s">
         <v>8</v>
       </c>
       <c r="E4" s="8" t="s">
@@ -1246,38 +1251,38 @@
       <c r="F4" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="G4" s="13" t="s">
+      <c r="G4" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="H4" s="13" t="s">
+      <c r="H4" s="11" t="s">
         <v>10</v>
       </c>
       <c r="I4" s="8"/>
     </row>
     <row r="5" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A5" s="19"/>
-      <c r="B5" s="26"/>
-      <c r="C5" s="12"/>
-      <c r="D5" s="12"/>
+      <c r="A5" s="17"/>
+      <c r="B5" s="15"/>
+      <c r="C5" s="22"/>
+      <c r="D5" s="22"/>
       <c r="E5" s="9" t="s">
         <v>9</v>
       </c>
       <c r="F5" s="10" t="s">
-        <v>35</v>
-      </c>
-      <c r="G5" s="14"/>
-      <c r="H5" s="14"/>
+        <v>34</v>
+      </c>
+      <c r="G5" s="12"/>
+      <c r="H5" s="12"/>
       <c r="I5" s="1" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="6" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A6" s="19"/>
-      <c r="B6" s="26"/>
-      <c r="C6" s="11" t="s">
+      <c r="A6" s="17"/>
+      <c r="B6" s="15"/>
+      <c r="C6" s="21" t="s">
         <v>12</v>
       </c>
-      <c r="D6" s="11" t="s">
+      <c r="D6" s="21" t="s">
         <v>8</v>
       </c>
       <c r="E6" s="7" t="s">
@@ -1286,42 +1291,42 @@
       <c r="F6" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="G6" s="13" t="s">
+      <c r="G6" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="H6" s="13" t="s">
+      <c r="H6" s="11" t="s">
         <v>10</v>
       </c>
       <c r="I6" s="8"/>
     </row>
     <row r="7" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A7" s="20"/>
-      <c r="B7" s="16"/>
-      <c r="C7" s="12"/>
-      <c r="D7" s="12"/>
+      <c r="A7" s="18"/>
+      <c r="B7" s="14"/>
+      <c r="C7" s="22"/>
+      <c r="D7" s="22"/>
       <c r="E7" s="10" t="s">
         <v>22</v>
       </c>
       <c r="F7" s="10" t="s">
-        <v>35</v>
-      </c>
-      <c r="G7" s="14"/>
-      <c r="H7" s="14"/>
+        <v>34</v>
+      </c>
+      <c r="G7" s="12"/>
+      <c r="H7" s="12"/>
       <c r="I7" s="1" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="8" spans="1:9" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="17" t="s">
+      <c r="A8" s="23" t="s">
         <v>13</v>
       </c>
-      <c r="B8" s="17" t="s">
+      <c r="B8" s="23" t="s">
         <v>14</v>
       </c>
-      <c r="C8" s="11" t="s">
+      <c r="C8" s="21" t="s">
         <v>7</v>
       </c>
-      <c r="D8" s="11" t="s">
+      <c r="D8" s="21" t="s">
         <v>8</v>
       </c>
       <c r="E8" s="1" t="s">
@@ -1330,38 +1335,38 @@
       <c r="F8" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="G8" s="13" t="s">
+      <c r="G8" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="H8" s="15" t="s">
+      <c r="H8" s="13" t="s">
         <v>21</v>
       </c>
-      <c r="I8" s="13" t="s">
+      <c r="I8" s="11" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="9" spans="1:9" ht="32.549999999999997" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="17"/>
-      <c r="B9" s="17"/>
-      <c r="C9" s="12"/>
-      <c r="D9" s="12"/>
+      <c r="A9" s="23"/>
+      <c r="B9" s="23"/>
+      <c r="C9" s="22"/>
+      <c r="D9" s="22"/>
       <c r="E9" s="5" t="s">
         <v>9</v>
       </c>
       <c r="F9" s="6" t="s">
-        <v>35</v>
-      </c>
-      <c r="G9" s="14"/>
-      <c r="H9" s="16"/>
-      <c r="I9" s="14"/>
+        <v>34</v>
+      </c>
+      <c r="G9" s="12"/>
+      <c r="H9" s="14"/>
+      <c r="I9" s="12"/>
     </row>
     <row r="10" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A10" s="17"/>
-      <c r="B10" s="17"/>
-      <c r="C10" s="11" t="s">
+      <c r="A10" s="23"/>
+      <c r="B10" s="23"/>
+      <c r="C10" s="21" t="s">
         <v>11</v>
       </c>
-      <c r="D10" s="11" t="s">
+      <c r="D10" s="21" t="s">
         <v>8</v>
       </c>
       <c r="E10" s="4" t="s">
@@ -1370,38 +1375,38 @@
       <c r="F10" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="G10" s="13" t="s">
+      <c r="G10" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="H10" s="15" t="s">
+      <c r="H10" s="13" t="s">
         <v>21</v>
       </c>
       <c r="I10" s="2"/>
     </row>
     <row r="11" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A11" s="17"/>
-      <c r="B11" s="17"/>
-      <c r="C11" s="12"/>
-      <c r="D11" s="12"/>
+      <c r="A11" s="23"/>
+      <c r="B11" s="23"/>
+      <c r="C11" s="22"/>
+      <c r="D11" s="22"/>
       <c r="E11" s="6" t="s">
         <v>23</v>
       </c>
       <c r="F11" s="6" t="s">
-        <v>35</v>
-      </c>
-      <c r="G11" s="14"/>
-      <c r="H11" s="16"/>
+        <v>34</v>
+      </c>
+      <c r="G11" s="12"/>
+      <c r="H11" s="14"/>
       <c r="I11" s="1" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A12" s="17"/>
-      <c r="B12" s="17"/>
-      <c r="C12" s="11" t="s">
+      <c r="A12" s="23"/>
+      <c r="B12" s="23"/>
+      <c r="C12" s="21" t="s">
         <v>12</v>
       </c>
-      <c r="D12" s="11" t="s">
+      <c r="D12" s="21" t="s">
         <v>8</v>
       </c>
       <c r="E12" s="3" t="s">
@@ -1410,39 +1415,39 @@
       <c r="F12" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="G12" s="13" t="s">
+      <c r="G12" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="H12" s="15" t="s">
+      <c r="H12" s="13" t="s">
         <v>21</v>
       </c>
       <c r="I12" s="3"/>
     </row>
     <row r="13" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A13" s="17"/>
-      <c r="B13" s="17"/>
-      <c r="C13" s="12"/>
-      <c r="D13" s="12"/>
+      <c r="A13" s="23"/>
+      <c r="B13" s="23"/>
+      <c r="C13" s="22"/>
+      <c r="D13" s="22"/>
       <c r="E13" s="5" t="s">
         <v>15</v>
       </c>
       <c r="F13" s="6" t="s">
-        <v>35</v>
-      </c>
-      <c r="G13" s="14"/>
-      <c r="H13" s="16"/>
+        <v>34</v>
+      </c>
+      <c r="G13" s="12"/>
+      <c r="H13" s="14"/>
       <c r="I13" s="1" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A14" s="18" t="s">
+      <c r="A14" s="16" t="s">
         <v>16</v>
       </c>
-      <c r="B14" s="21" t="s">
-        <v>31</v>
-      </c>
-      <c r="C14" s="13" t="s">
+      <c r="B14" s="24" t="s">
+        <v>38</v>
+      </c>
+      <c r="C14" s="11" t="s">
         <v>7</v>
       </c>
       <c r="D14" s="1" t="s">
@@ -1451,31 +1456,31 @@
       <c r="E14" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="F14" s="24" t="s">
-        <v>36</v>
-      </c>
-      <c r="G14" s="13"/>
-      <c r="H14" s="15"/>
-      <c r="I14" s="13"/>
+      <c r="F14" s="19" t="s">
+        <v>35</v>
+      </c>
+      <c r="G14" s="11"/>
+      <c r="H14" s="13"/>
+      <c r="I14" s="11"/>
     </row>
     <row r="15" spans="1:9" ht="28.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="19"/>
-      <c r="B15" s="22"/>
-      <c r="C15" s="14"/>
+      <c r="A15" s="17"/>
+      <c r="B15" s="25"/>
+      <c r="C15" s="12"/>
       <c r="D15" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="E15" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="E15" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="F15" s="25"/>
-      <c r="G15" s="14"/>
-      <c r="H15" s="16"/>
-      <c r="I15" s="14"/>
+      <c r="F15" s="20"/>
+      <c r="G15" s="12"/>
+      <c r="H15" s="14"/>
+      <c r="I15" s="12"/>
     </row>
     <row r="16" spans="1:9" ht="46.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="19"/>
-      <c r="B16" s="22"/>
+      <c r="A16" s="17"/>
+      <c r="B16" s="25"/>
       <c r="C16" s="1" t="s">
         <v>11</v>
       </c>
@@ -1486,36 +1491,36 @@
         <v>28</v>
       </c>
       <c r="F16" s="5" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="G16" s="1"/>
       <c r="H16" s="1"/>
       <c r="I16" s="1"/>
     </row>
-    <row r="17" spans="1:9" ht="60" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="20"/>
-      <c r="B17" s="23"/>
+    <row r="17" spans="1:9" ht="69.599999999999994" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="18"/>
+      <c r="B17" s="26"/>
       <c r="C17" s="1" t="s">
         <v>12</v>
       </c>
       <c r="D17" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="E17" s="1" t="s">
-        <v>15</v>
+      <c r="E17" s="7" t="s">
+        <v>37</v>
       </c>
       <c r="F17" s="5" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="G17" s="1"/>
       <c r="H17" s="1"/>
       <c r="I17" s="1"/>
     </row>
     <row r="18" spans="1:9" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A18" s="17" t="s">
+      <c r="A18" s="23" t="s">
         <v>18</v>
       </c>
-      <c r="B18" s="17" t="s">
+      <c r="B18" s="23" t="s">
         <v>19</v>
       </c>
       <c r="C18" s="1" t="s">
@@ -1534,15 +1539,15 @@
         <v>29</v>
       </c>
       <c r="H18" s="4" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="I18" s="1" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A19" s="17"/>
-      <c r="B19" s="17"/>
+      <c r="A19" s="23"/>
+      <c r="B19" s="23"/>
       <c r="C19" s="1" t="s">
         <v>11</v>
       </c>
@@ -1554,8 +1559,8 @@
       <c r="I19" s="1"/>
     </row>
     <row r="20" spans="1:9" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A20" s="17"/>
-      <c r="B20" s="17"/>
+      <c r="A20" s="23"/>
+      <c r="B20" s="23"/>
       <c r="C20" s="1" t="s">
         <v>12</v>
       </c>
@@ -1572,7 +1577,7 @@
         <v>30</v>
       </c>
       <c r="H20" s="4" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="I20" s="1" t="s">
         <v>25</v>
@@ -1581,6 +1586,28 @@
   </sheetData>
   <autoFilter ref="A1:I1" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
   <mergeCells count="38">
+    <mergeCell ref="D2:D3"/>
+    <mergeCell ref="C6:C7"/>
+    <mergeCell ref="D6:D7"/>
+    <mergeCell ref="I8:I9"/>
+    <mergeCell ref="B8:B13"/>
+    <mergeCell ref="C10:C11"/>
+    <mergeCell ref="D10:D11"/>
+    <mergeCell ref="C12:C13"/>
+    <mergeCell ref="D12:D13"/>
+    <mergeCell ref="C8:C9"/>
+    <mergeCell ref="D8:D9"/>
+    <mergeCell ref="B18:B20"/>
+    <mergeCell ref="A8:A13"/>
+    <mergeCell ref="A18:A20"/>
+    <mergeCell ref="B14:B17"/>
+    <mergeCell ref="A2:A7"/>
+    <mergeCell ref="H14:H15"/>
+    <mergeCell ref="I14:I15"/>
+    <mergeCell ref="C14:C15"/>
+    <mergeCell ref="A14:A17"/>
+    <mergeCell ref="F14:F15"/>
+    <mergeCell ref="G14:G15"/>
     <mergeCell ref="G10:G11"/>
     <mergeCell ref="H10:H11"/>
     <mergeCell ref="G12:G13"/>
@@ -1592,33 +1619,11 @@
     <mergeCell ref="H2:H3"/>
     <mergeCell ref="H4:H5"/>
     <mergeCell ref="H6:H7"/>
-    <mergeCell ref="H14:H15"/>
-    <mergeCell ref="I14:I15"/>
-    <mergeCell ref="C14:C15"/>
-    <mergeCell ref="A14:A17"/>
-    <mergeCell ref="F14:F15"/>
-    <mergeCell ref="G14:G15"/>
     <mergeCell ref="C4:C5"/>
-    <mergeCell ref="B18:B20"/>
-    <mergeCell ref="A8:A13"/>
-    <mergeCell ref="A18:A20"/>
-    <mergeCell ref="B14:B17"/>
-    <mergeCell ref="A2:A7"/>
     <mergeCell ref="D4:D5"/>
     <mergeCell ref="G8:G9"/>
     <mergeCell ref="H8:H9"/>
-    <mergeCell ref="I8:I9"/>
-    <mergeCell ref="B8:B13"/>
-    <mergeCell ref="C10:C11"/>
-    <mergeCell ref="D10:D11"/>
-    <mergeCell ref="C12:C13"/>
-    <mergeCell ref="D12:D13"/>
-    <mergeCell ref="C8:C9"/>
-    <mergeCell ref="D8:D9"/>
     <mergeCell ref="C2:C3"/>
-    <mergeCell ref="D2:D3"/>
-    <mergeCell ref="C6:C7"/>
-    <mergeCell ref="D6:D7"/>
   </mergeCells>
   <phoneticPr fontId="18" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>